<commit_message>
Arbeit: Absatz 2.3.1 (Versuch) fertig
</commit_message>
<xml_diff>
--- a/Messungen/ImFreien/Messergebnisse.xlsx
+++ b/Messungen/ImFreien/Messergebnisse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Levin\Schule\JugendForscht\Messungen\ImFreien\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D812955-7554-4E0B-83F6-E336FEC43F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE479C2B-B0EE-4E5D-88BE-FBB6EC808E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{7730BCC9-650B-44A2-BA96-52B856EA7E52}"/>
+    <workbookView xWindow="57480" yWindow="14520" windowWidth="29040" windowHeight="15840" xr2:uid="{7730BCC9-650B-44A2-BA96-52B856EA7E52}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -227,20 +219,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="5"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="7"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="6"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="5"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -2862,16 +2854,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>374650</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>635001</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>76253</xdr:rowOff>
+      <xdr:rowOff>92128</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2898,16 +2890,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>369886</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>230186</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>87125</xdr:rowOff>
+      <xdr:rowOff>103000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>44450</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3224,7 +3216,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3235,7 +3227,7 @@
   <dimension ref="C5:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N31" sqref="N31"/>
+      <selection activeCell="H7" sqref="H7:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3244,15 +3236,15 @@
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="3:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="D5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="3:6" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C6" s="4" t="s">
+    <row r="6" spans="3:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D6" t="s">
@@ -3265,7 +3257,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C7">
         <v>0.6</v>
       </c>
@@ -3278,8 +3270,12 @@
       <c r="F7">
         <v>-14.368399999999999</v>
       </c>
+      <c r="H7">
+        <f>AVERAGE(D7:F7)</f>
+        <v>-13.512766666666666</v>
+      </c>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C8">
         <v>1</v>
       </c>
@@ -3292,8 +3288,12 @@
       <c r="F8">
         <v>-18.5245</v>
       </c>
+      <c r="H8">
+        <f>AVERAGE(D8:F8)</f>
+        <v>-18.215999999999998</v>
+      </c>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C9">
         <v>1.25</v>
       </c>
@@ -3306,8 +3306,12 @@
       <c r="F9">
         <v>-21.163799999999998</v>
       </c>
+      <c r="H9">
+        <f>AVERAGE(D9:F9)</f>
+        <v>-20.603399999999997</v>
+      </c>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C10">
         <v>1.5</v>
       </c>
@@ -3320,8 +3324,12 @@
       <c r="F10">
         <v>-23.190100000000001</v>
       </c>
+      <c r="H10">
+        <f>AVERAGE(D10:F10)</f>
+        <v>-22.3796</v>
+      </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C11">
         <v>2</v>
       </c>
@@ -3334,8 +3342,12 @@
       <c r="F11">
         <v>-25.863399999999999</v>
       </c>
+      <c r="H11">
+        <f>AVERAGE(D11:F11)</f>
+        <v>-25.010400000000001</v>
+      </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C12">
         <v>2.5</v>
       </c>
@@ -3348,8 +3360,12 @@
       <c r="F12">
         <v>-27.6037</v>
       </c>
+      <c r="H12">
+        <f>AVERAGE(D12:F12)</f>
+        <v>-25.762366666666665</v>
+      </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.35">
       <c r="C13">
         <v>3</v>
       </c>
@@ -3362,16 +3378,20 @@
       <c r="F13" s="1">
         <v>-22.6935</v>
       </c>
+      <c r="H13">
+        <f>AVERAGE(D13:F13)</f>
+        <v>-26.896733333333334</v>
+      </c>
     </row>
     <row r="18" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
     </row>
     <row r="19" spans="3:7" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D19" t="s">
@@ -3504,33 +3524,33 @@
       </c>
     </row>
     <row r="30" spans="3:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31" spans="3:7" ht="15.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
     </row>
     <row r="32" spans="3:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E32" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E33" t="s">
@@ -3542,10 +3562,10 @@
       <c r="G33" t="s">
         <v>4</v>
       </c>
-      <c r="H33" s="9" t="s">
+      <c r="H33" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3634,12 +3654,12 @@
       </c>
     </row>
     <row r="38" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="I38" s="8" t="s">
+      <c r="I38" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="39" spans="3:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="I39" s="10">
+      <c r="I39" s="7">
         <f>AVERAGE(I34:I36)</f>
         <v>-6.4140333333333324</v>
       </c>
@@ -3652,6 +3672,16 @@
     <mergeCell ref="C30:G31"/>
   </mergeCells>
   <conditionalFormatting sqref="E34:G36">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="-6"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFF9900"/>
+      </colorScale>
+    </cfRule>
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -3662,18 +3692,11 @@
         <color rgb="FFFFC000"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="num" val="-6"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FF92D050"/>
-        <color rgb="FFFF9900"/>
-      </colorScale>
-    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="H7 H8:H13" formulaRange="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>